<commit_message>
update to figures and table
</commit_message>
<xml_diff>
--- a/RO_polls_presidential_2019.xlsx
+++ b/RO_polls_presidential_2019.xlsx
@@ -5,27 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borbath\Documents\GitHub\ro_poll_pres_2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\borbath\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD043AFC-212E-4DD9-80D5-2A75B0DC1A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0667AB83-511B-4ED2-B29B-CEA5352ACF5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="167" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="67">
   <si>
     <t>Polling company</t>
   </si>
@@ -171,10 +179,61 @@
     <t>https://www.romaniatv.net/sondaj-sociopol-prezidentiale-2019-finala-intre-klaus-iohannis-si-viorica-dancila_493039.html</t>
   </si>
   <si>
-    <t>subsample analysis</t>
-  </si>
-  <si>
     <t>Alexandru Cumpănasu</t>
+  </si>
+  <si>
+    <t>The poll also had Tariceanu (13.8),  Ponta (12.9),  Ciolos (10.4), Eugen Tomac (1.5) - none of them ended up running</t>
+  </si>
+  <si>
+    <t>The poll also had Tariceanu (18), and other candidates (8)</t>
+  </si>
+  <si>
+    <t>The poll also had Tariceanu (12.7), Ponta (14), Tomac (0.6)</t>
+  </si>
+  <si>
+    <t>Other candidates</t>
+  </si>
+  <si>
+    <t>for some reason the sum is 102 percent, probably due to rounding error in publishing the result</t>
+  </si>
+  <si>
+    <t>The sum of the preferences is only 96 percent, probably due to not having the preferences for other candidates reported</t>
+  </si>
+  <si>
+    <t>The sum of the preferences is only 97 percent, probably due to not having the preferences for other candidates reported</t>
+  </si>
+  <si>
+    <t>only second round preferences, not including those who have no preferences (27.5) or would not vote (6)</t>
+  </si>
+  <si>
+    <t>only second round preferences, not including those who have no preferences (27.4) or would not vote (8.8)</t>
+  </si>
+  <si>
+    <t>Not included in the calculations</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Intervals and not exact numbers are reported. The table has the mean of the intervals reported: Dancila (18-22), Paleologu (7-9)</t>
+  </si>
+  <si>
+    <t>The sum of the preferences is only 94 percent, probably due to not having the preferences for other candidates reported</t>
+  </si>
+  <si>
+    <t>The sum of the preferences is only 81 percent, probably at least partly due to missing data for the other candidates</t>
+  </si>
+  <si>
+    <t>The sum of the preferences is only 96 percent, probably due to rounding error</t>
+  </si>
+  <si>
+    <t>subsample analysis of PNL, USR, PLUS voters only, also includes Ciolos (15), Rares Bogdan (9.6), Chichirau (0.8), Vlad Voiculescu (5), no vote (0.8), don't know (1.9)</t>
+  </si>
+  <si>
+    <t>subsample analysis of PSD, ALDE, PRO Romania voters only, also includes Firea (23.3), Ponta (20.6), Tariceanu (9.1), Plesoianu (7.9), no vote (0.7), don't know (4.9)</t>
+  </si>
+  <si>
+    <t>The sum of preferences is only 83 percent, probably because of missing the poll numbers for the candidates not reported.</t>
   </si>
 </sst>
 </file>
@@ -214,18 +273,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -250,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -271,7 +324,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -565,34 +617,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G11" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomRight" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.21875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="11" style="6" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" style="1" customWidth="1"/>
-    <col min="7" max="10" width="9.21875" style="7"/>
-    <col min="11" max="11" width="9.77734375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="9.21875" style="7"/>
-    <col min="13" max="13" width="11.21875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="9.21875" style="7"/>
-    <col min="15" max="15" width="151.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.77734375" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="9.21875" style="5"/>
+    <col min="4" max="4" width="12.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="9.33203125" style="7"/>
+    <col min="11" max="11" width="9.6640625" style="7" customWidth="1"/>
+    <col min="12" max="13" width="9.33203125" style="7"/>
+    <col min="14" max="14" width="11.33203125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="7"/>
+    <col min="16" max="16" width="151.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="106.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.33203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="2" customFormat="1" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -630,19 +682,25 @@
         <v>13</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="R1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>19</v>
       </c>
@@ -673,11 +731,17 @@
       <c r="L2" s="7">
         <v>2.8</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="M2" s="7">
+        <v>38.6</v>
+      </c>
+      <c r="P2" s="9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>19</v>
       </c>
@@ -708,11 +772,17 @@
       <c r="L3" s="7">
         <v>4</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="M3" s="7">
+        <v>26</v>
+      </c>
+      <c r="P3" s="9" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q3" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>19</v>
       </c>
@@ -740,11 +810,17 @@
       <c r="L4" s="7">
         <v>2.4</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="M4" s="7">
+        <v>27.3</v>
+      </c>
+      <c r="P4" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>37</v>
       </c>
@@ -781,11 +857,17 @@
       <c r="L5" s="7">
         <v>1</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="M5" s="7">
+        <v>3</v>
+      </c>
+      <c r="P5" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q5" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
@@ -822,11 +904,14 @@
       <c r="L6" s="7">
         <v>1</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="M6" s="7">
+        <v>3</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -851,14 +936,17 @@
       <c r="I7" s="7">
         <v>35</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="P7" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="Q7" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
@@ -895,11 +983,14 @@
       <c r="L8" s="7">
         <v>3</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="M8" s="7">
+        <v>2</v>
+      </c>
+      <c r="P8" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -936,11 +1027,14 @@
       <c r="L9" s="7">
         <v>2</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="M9" s="7">
+        <v>6</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -977,14 +1071,14 @@
       <c r="L10" s="7">
         <v>3</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="11" t="s">
+      <c r="M10" s="7">
+        <v>2</v>
+      </c>
+      <c r="P10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>43711</v>
       </c>
@@ -1015,357 +1109,369 @@
       <c r="L11" s="7">
         <v>3.1</v>
       </c>
-      <c r="O11" s="9" t="s">
+      <c r="P11" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="Q11" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
+        <v>43711</v>
+      </c>
+      <c r="C12" s="6">
+        <v>43732</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G12" s="7">
+        <v>44.2</v>
+      </c>
+      <c r="J12" s="7">
+        <v>22.2</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B13" s="6">
         <v>43717</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C13" s="6">
         <v>43736</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>1010</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G13" s="7">
         <v>45.3</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="7">
         <v>16.600000000000001</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I13" s="7">
         <v>12.4</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J13" s="7">
         <v>14.2</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K13" s="7">
         <v>7.7</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L13" s="7">
         <v>3.8</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C13" s="6">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C14" s="6">
         <v>43742</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G14" s="7">
         <v>40</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H14" s="7">
         <v>13</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I14" s="7">
+        <v>20</v>
+      </c>
+      <c r="J14" s="7">
+        <v>20</v>
+      </c>
+      <c r="K14" s="7">
+        <v>8</v>
+      </c>
+      <c r="P14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43744</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="7">
-        <v>20</v>
-      </c>
-      <c r="K13" s="7">
+      <c r="G15" s="7">
+        <v>43</v>
+      </c>
+      <c r="H15" s="7">
+        <v>11</v>
+      </c>
+      <c r="I15" s="7">
+        <v>21</v>
+      </c>
+      <c r="J15" s="7">
+        <v>15</v>
+      </c>
+      <c r="K15" s="7">
+        <v>4</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C16" s="6">
+        <v>43755</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="7">
+        <v>40</v>
+      </c>
+      <c r="H16" s="7">
         <v>9</v>
       </c>
-      <c r="O13" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6">
-        <v>43744</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="7">
-        <v>43</v>
-      </c>
-      <c r="H14" s="7">
-        <v>11</v>
-      </c>
-      <c r="I14" s="7">
-        <v>21</v>
-      </c>
-      <c r="J14" s="7">
-        <v>15</v>
-      </c>
-      <c r="K14" s="7">
-        <v>4</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C15" s="6">
-        <v>43755</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="7">
-        <v>40</v>
-      </c>
-      <c r="H15" s="7">
-        <v>9</v>
-      </c>
-      <c r="I15" s="7">
+      <c r="I16" s="7">
         <v>13</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J16" s="7">
         <v>12</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K16" s="7">
         <v>7</v>
       </c>
-      <c r="O15" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="6">
-        <v>43752</v>
-      </c>
-      <c r="C16" s="6">
-        <v>43759</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1600</v>
-      </c>
-      <c r="G16" s="7">
-        <v>37</v>
-      </c>
-      <c r="H16" s="7">
-        <v>11</v>
-      </c>
-      <c r="I16" s="7">
-        <v>20</v>
-      </c>
-      <c r="J16" s="7">
-        <v>13</v>
-      </c>
-      <c r="K16" s="7">
-        <v>6</v>
-      </c>
-      <c r="L16" s="7">
-        <v>4</v>
-      </c>
-      <c r="M16" s="7">
-        <v>4</v>
-      </c>
-      <c r="N16" s="7">
-        <v>4</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q16" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="6">
+        <v>43752</v>
+      </c>
+      <c r="C17" s="6">
+        <v>43759</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1600</v>
+      </c>
+      <c r="G17" s="7">
+        <v>37</v>
+      </c>
+      <c r="H17" s="7">
+        <v>11</v>
+      </c>
+      <c r="I17" s="7">
+        <v>20</v>
+      </c>
+      <c r="J17" s="7">
+        <v>13</v>
+      </c>
+      <c r="K17" s="7">
+        <v>6</v>
+      </c>
+      <c r="L17" s="7">
+        <v>4</v>
+      </c>
+      <c r="M17" s="7">
+        <v>1</v>
+      </c>
+      <c r="N17" s="7">
+        <v>4</v>
+      </c>
+      <c r="O17" s="7">
+        <v>4</v>
+      </c>
+      <c r="P17" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="6">
         <v>43749</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C18" s="6">
         <v>43760</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F18" s="1">
         <v>1001</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G18" s="7">
         <v>42</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H18" s="7">
         <v>10</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I18" s="7">
         <v>21</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J18" s="7">
         <v>10</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="P18" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="6">
+      <c r="Q18" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B19" s="6">
         <v>43753</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C19" s="6">
         <v>43761</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <v>2000</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G19" s="7">
         <v>39</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H19" s="7">
         <v>8</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I19" s="7">
         <v>23.4</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J19" s="7">
         <v>18.5</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K19" s="7">
         <v>3.8</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L19" s="7">
         <v>3.9</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="P19" s="9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C19" s="6">
+      <c r="Q19" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="6">
+        <v>43753</v>
+      </c>
+      <c r="C20" s="6">
+        <v>43761</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G20" s="7">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="J20" s="7">
+        <v>24</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C21" s="6">
         <v>43765</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G21" s="7">
         <v>40</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H21" s="7">
         <v>7</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I21" s="7">
         <v>19</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J21" s="7">
         <v>13</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K21" s="7">
         <v>8</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L21" s="7">
         <v>4</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M21" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="N21" s="7">
         <v>3</v>
       </c>
-      <c r="O19" s="9" t="s">
+      <c r="P21" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="Q21" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" s="6">
-        <v>43746</v>
-      </c>
-      <c r="C20" s="6">
-        <v>43766</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1010</v>
-      </c>
-      <c r="G20" s="7">
-        <v>45.7</v>
-      </c>
-      <c r="H20" s="7">
-        <v>16.7</v>
-      </c>
-      <c r="I20" s="7">
-        <v>15.1</v>
-      </c>
-      <c r="J20" s="7">
-        <v>12.6</v>
-      </c>
-      <c r="K20" s="7">
-        <v>6.9</v>
-      </c>
-      <c r="L20" s="7">
-        <v>2.9</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="6">
-        <v>43746</v>
-      </c>
-      <c r="C21" s="6">
-        <v>43766</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="1">
-        <v>1010</v>
-      </c>
-      <c r="H21" s="7">
-        <v>12.1</v>
-      </c>
-      <c r="I21" s="7">
-        <v>24.5</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P21" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="B22" s="6">
         <v>43746</v>
@@ -1383,46 +1489,134 @@
         <v>1010</v>
       </c>
       <c r="G22" s="7">
+        <v>45.7</v>
+      </c>
+      <c r="H22" s="7">
+        <v>16.7</v>
+      </c>
+      <c r="I22" s="7">
+        <v>15.1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>12.6</v>
+      </c>
+      <c r="K22" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="L22" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="6">
+        <v>43746</v>
+      </c>
+      <c r="C23" s="6">
+        <v>43766</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1010</v>
+      </c>
+      <c r="H23" s="7">
+        <v>12.1</v>
+      </c>
+      <c r="I23" s="7">
+        <v>24.5</v>
+      </c>
+      <c r="M23" s="7">
+        <v>60.9</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="6">
+        <v>43746</v>
+      </c>
+      <c r="C24" s="6">
+        <v>43766</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1010</v>
+      </c>
+      <c r="G24" s="7">
         <v>52.6</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J24" s="7">
         <v>14.3</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="M24" s="7">
+        <v>30.4</v>
+      </c>
+      <c r="P24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P22" s="5" t="s">
-        <v>48</v>
+      <c r="Q24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P22">
-    <sortCondition ref="C2:C22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q24">
+    <sortCondition ref="C2:C24"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="O20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="O3:O4" r:id="rId2" display="https://www.europafm.ro/barometru-europa-fm-cum-ar-vota-romanii-daca-ar-fi-duminica-alegerile/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="O17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="O16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="O15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="O19" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="O11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="O12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="O18" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="O13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="O10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="O6" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="O4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="O3" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="O7" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="O2" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="O21" r:id="rId17" xr:uid="{5D9CCDE1-151A-4FCC-AEB7-C64D76B9770B}"/>
-    <hyperlink ref="O5" r:id="rId18" xr:uid="{E48CA84A-5AE1-4183-9E0F-076FEDDA0B28}"/>
-    <hyperlink ref="O8" r:id="rId19" xr:uid="{50751241-88F5-40C6-819B-9FFF7929DB90}"/>
-    <hyperlink ref="O9" r:id="rId20" xr:uid="{52C54887-9795-4D3C-B340-DB021661632B}"/>
-    <hyperlink ref="O22" r:id="rId21" xr:uid="{FB578C49-6DDD-45A7-A4C4-7E3108235E1A}"/>
+    <hyperlink ref="P22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="P3:P4" r:id="rId2" display="https://www.europafm.ro/barometru-europa-fm-cum-ar-vota-romanii-daca-ar-fi-duminica-alegerile/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="P18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="P17" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="P16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="P21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="P11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="P13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="P19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="P14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="P10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="P6" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="P4" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="P3" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="P7" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="P2" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="P23" r:id="rId17" xr:uid="{5D9CCDE1-151A-4FCC-AEB7-C64D76B9770B}"/>
+    <hyperlink ref="P5" r:id="rId18" xr:uid="{E48CA84A-5AE1-4183-9E0F-076FEDDA0B28}"/>
+    <hyperlink ref="P8" r:id="rId19" xr:uid="{50751241-88F5-40C6-819B-9FFF7929DB90}"/>
+    <hyperlink ref="P9" r:id="rId20" xr:uid="{52C54887-9795-4D3C-B340-DB021661632B}"/>
+    <hyperlink ref="P24" r:id="rId21" xr:uid="{FB578C49-6DDD-45A7-A4C4-7E3108235E1A}"/>
+    <hyperlink ref="P12" r:id="rId22" xr:uid="{28D1F718-D0D9-49D8-A5C4-F0BB8D3A23AE}"/>
+    <hyperlink ref="P20" r:id="rId23" xr:uid="{B2AB7C49-9DA5-4FDE-9466-A4FA238316DC}"/>
+    <hyperlink ref="P15" r:id="rId24" xr:uid="{450E0341-C271-4A30-B143-D0DDA1270059}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId22"/>
+  <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>